<commit_message>
Add plus signs and fix about
</commit_message>
<xml_diff>
--- a/test/fixtures/success.xlsx
+++ b/test/fixtures/success.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5840" yWindow="900" windowWidth="25120" windowHeight="15840" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,7 +432,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -445,10 +445,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">

</xml_diff>